<commit_message>
menambahkan halaman application settings
</commit_message>
<xml_diff>
--- a/public/testing.xlsx
+++ b/public/testing.xlsx
@@ -75,16 +75,16 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Garamond"/>
     </font>
     <font>
       <b val="1"/>
-      <i val="0"/>
+      <i val="1"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,10 +424,10 @@
   <cols>
     <col min="1" max="1" width="30.421" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="16.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="24.565" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="24.565" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="24.565" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="26.279" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="26.279" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="26.279" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>